<commit_message>
division par 100 sur excel
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GrégoireBERAUD\hackaton\PI-Recylage_Al\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F61F2B3-13C8-4C0D-808E-D397D011340F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB236C4-07EC-4E77-B470-607E60D43158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="site" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,20 @@
     <sheet name="currency" sheetId="5" r:id="rId5"/>
     <sheet name="external_scrap" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -831,7 +844,9 @@
   </sheetPr>
   <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -884,29 +899,29 @@
       <c r="B2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="F2" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="G2" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="H2" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="I2" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="J2" s="5">
-        <v>0.03</v>
+      <c r="C2" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D2" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E2" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F2" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G2" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H2" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I2" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="J2" s="8">
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="L2" s="4"/>
     </row>
@@ -917,29 +932,29 @@
       <c r="B3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.95</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.05</v>
+      <c r="C3" s="8">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="E3" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G3" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H3" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I3" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J3" s="8">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="L3" s="4"/>
     </row>
@@ -950,29 +965,29 @@
       <c r="B4" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="E4" s="6">
-        <v>4</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G4" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.15</v>
+      <c r="C4" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D4" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="F4" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G4" s="8">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="H4" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I4" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J4" s="8">
+        <v>1.5E-3</v>
       </c>
       <c r="L4" s="4"/>
     </row>
@@ -983,29 +998,29 @@
       <c r="B5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.05</v>
+      <c r="C5" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D5" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I5" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J5" s="8">
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="L5" s="4"/>
     </row>
@@ -1016,29 +1031,29 @@
       <c r="B6" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="D6" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E6" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2.4</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.15</v>
+      <c r="C6" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F6" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="G6" s="8">
+        <v>2.4E-2</v>
+      </c>
+      <c r="H6" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="I6" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J6" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1048,29 +1063,29 @@
       <c r="B7" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="D7" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E7" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G7" s="5">
-        <v>4.5</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0.15</v>
+      <c r="C7" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G7" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I7" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1080,29 +1095,29 @@
       <c r="B8" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.15</v>
+      <c r="C8" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="F8" s="8">
+        <v>1.5E-3</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H8" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="I8" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J8" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1112,29 +1127,29 @@
       <c r="B9" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.35</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F9" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.1</v>
+      <c r="C9" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D9" s="8">
+        <v>3.4999999999999996E-3</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F9" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I9" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J9" s="8">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1144,29 +1159,29 @@
       <c r="B10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="E10" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="F10" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="G10" s="5">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="H10" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I10" s="6">
-        <v>6</v>
-      </c>
-      <c r="J10" s="5">
-        <v>0.2</v>
+      <c r="C10" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F10" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G10" s="8">
+        <v>2.3E-2</v>
+      </c>
+      <c r="H10" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="I10" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="J10" s="8">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1176,29 +1191,29 @@
       <c r="B11" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="D11" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E11" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="H11" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="I11" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0.08</v>
+      <c r="C11" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="G11" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H11" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J11" s="8">
+        <v>8.0000000000000004E-4</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1208,29 +1223,29 @@
       <c r="B12" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E12" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="F12" s="5">
-        <v>1.3</v>
-      </c>
-      <c r="G12" s="6">
-        <v>1</v>
-      </c>
-      <c r="H12" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="I12" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0.05</v>
+      <c r="C12" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D12" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F12" s="8">
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H12" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I12" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J12" s="8">
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1240,29 +1255,29 @@
       <c r="B13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="D13" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E13" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G13" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="H13" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I13" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0.1</v>
+      <c r="C13" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D13" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F13" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G13" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H13" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="I13" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J13" s="8">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1272,29 +1287,29 @@
       <c r="B14" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E14" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="F14" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="G14" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="H14" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I14" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J14" s="5">
-        <v>0.1</v>
+      <c r="C14" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D14" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E14" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="F14" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="G14" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I14" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J14" s="8">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1304,29 +1319,29 @@
       <c r="B15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C15" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="D15" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G15" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="H15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I15" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="J15" s="5">
-        <v>0.1</v>
+      <c r="C15" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D15" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="G15" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="J15" s="8">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1336,29 +1351,29 @@
       <c r="B16" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="D16" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E16" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F16" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="G16" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="H16" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I16" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J16" s="5">
-        <v>0.2</v>
+      <c r="C16" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F16" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="G16" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I16" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J16" s="8">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1368,29 +1383,29 @@
       <c r="B17" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C17" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="D17" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="E17" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F17" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="G17" s="6">
-        <v>3</v>
-      </c>
-      <c r="H17" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="I17" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="J17" s="5">
-        <v>0.15</v>
+      <c r="C17" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D17" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F17" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="H17" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I17" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="J17" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1400,29 +1415,29 @@
       <c r="B18" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C18" s="5">
-        <v>0.4</v>
-      </c>
-      <c r="D18" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="E18" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F18" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="G18" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="H18" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="I18" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0.1</v>
+      <c r="C18" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D18" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="E18" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F18" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="G18" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H18" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I18" s="8">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J18" s="8">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1432,29 +1447,29 @@
       <c r="B19" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="D19" s="5">
-        <v>0.7</v>
-      </c>
-      <c r="E19" s="6">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="G19" s="6">
-        <v>1</v>
-      </c>
-      <c r="H19" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I19" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0.15</v>
+      <c r="C19" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D19" s="8">
+        <v>6.9999999999999993E-3</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="8">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I19" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1464,29 +1479,29 @@
       <c r="B20" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="E20" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="F20" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="G20" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="H20" s="5">
-        <v>0.03</v>
-      </c>
-      <c r="I20" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0.03</v>
+      <c r="C20" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="F20" s="8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G20" s="8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H20" s="8">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="I20" s="8">
+        <v>7.000000000000001E-4</v>
+      </c>
+      <c r="J20" s="8">
+        <v>2.9999999999999997E-4</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1496,29 +1511,29 @@
       <c r="B21" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C21" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="D21" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="E21" s="6">
-        <v>2</v>
-      </c>
-      <c r="F21" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="G21" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="H21" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="I21" s="6">
-        <v>7</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0.2</v>
+      <c r="C21" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="D21" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E21" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="F21" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="G21" s="8">
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="H21" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="I21" s="8">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J21" s="8">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1528,29 +1543,29 @@
       <c r="B22" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="5">
-        <v>0.26</v>
-      </c>
-      <c r="D22" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="E22" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="F22" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="G22" s="5">
-        <v>2.5</v>
-      </c>
-      <c r="H22" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I22" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J22" s="5">
-        <v>0.2</v>
+      <c r="C22" s="8">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="D22" s="8">
+        <v>4.5000000000000005E-3</v>
+      </c>
+      <c r="E22" s="8">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F22" s="8">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G22" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H22" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I22" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J22" s="8">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1560,29 +1575,29 @@
       <c r="B23" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="D23" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="E23" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="F23" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="G23" s="5">
-        <v>3.1</v>
-      </c>
-      <c r="H23" s="5">
-        <v>0.3</v>
-      </c>
-      <c r="I23" s="5">
-        <v>0.2</v>
-      </c>
-      <c r="J23" s="5">
-        <v>0.15</v>
+      <c r="C23" s="8">
+        <v>4.5000000000000005E-3</v>
+      </c>
+      <c r="D23" s="8">
+        <v>4.5000000000000005E-3</v>
+      </c>
+      <c r="E23" s="8">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F23" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G23" s="8">
+        <v>3.1E-2</v>
+      </c>
+      <c r="H23" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I23" s="8">
+        <v>2E-3</v>
+      </c>
+      <c r="J23" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1592,29 +1607,29 @@
       <c r="B24" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="5">
-        <v>0.45</v>
-      </c>
-      <c r="D24" s="5">
-        <v>0.22</v>
-      </c>
-      <c r="E24" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="F24" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="G24" s="5">
-        <v>0.5</v>
-      </c>
-      <c r="H24" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="I24" s="5">
-        <v>0.15</v>
-      </c>
-      <c r="J24" s="5">
-        <v>0.1</v>
+      <c r="C24" s="8">
+        <v>4.5000000000000005E-3</v>
+      </c>
+      <c r="D24" s="8">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="F24" s="8">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G24" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H24" s="8">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="I24" s="8">
+        <v>1.5E-3</v>
+      </c>
+      <c r="J24" s="8">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1624,29 +1639,29 @@
       <c r="B25" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="5">
-        <v>0.6</v>
-      </c>
-      <c r="D25" s="5">
-        <v>0.75</v>
-      </c>
-      <c r="E25" s="5">
-        <v>1.2</v>
-      </c>
-      <c r="F25" s="5">
-        <v>0.9</v>
-      </c>
-      <c r="G25" s="6">
-        <v>1</v>
-      </c>
-      <c r="H25" s="5">
-        <v>0.1</v>
-      </c>
-      <c r="I25" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="J25" s="5">
-        <v>0.15</v>
+      <c r="C25" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D25" s="8">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="E25" s="8">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F25" s="8">
+        <v>9.0000000000000011E-3</v>
+      </c>
+      <c r="G25" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="H25" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="I25" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="J25" s="8">
+        <v>1.5E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2094,7 +2109,7 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>